<commit_message>
Further down the knit.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/NPS2025/DoD_2025_Prelim.xlsx
+++ b/Output/AcqTrends/NPS2025/DoD_2025_Prelim.xlsx
@@ -240,7 +240,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
-    <numFmt numFmtId="193" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="194" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="170" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="171" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="192" formatCode="0.00,,,&quot;B&quot;"/>
@@ -248,7 +248,7 @@
     <numFmt numFmtId="189" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="185" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="191" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="194" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="195" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -286,7 +286,7 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="193" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="194" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -295,7 +295,7 @@
     <xf numFmtId="189" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="185" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="194" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
Completed knit of acquisition_def.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/NPS2025/DoD_2025_Prelim.xlsx
+++ b/Output/AcqTrends/NPS2025/DoD_2025_Prelim.xlsx
@@ -240,7 +240,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
-    <numFmt numFmtId="194" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="195" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="170" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="171" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="192" formatCode="0.00,,,&quot;B&quot;"/>
@@ -248,7 +248,7 @@
     <numFmt numFmtId="189" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="185" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="191" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="195" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="196" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -286,7 +286,7 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="194" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="195" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
@@ -295,7 +295,7 @@
     <xf numFmtId="189" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="185" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="195" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="196" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>